<commit_message>
Commented out RT scoring for now. Added NTA result files.
</commit_message>
<xml_diff>
--- a/Code Time Estimation.xlsx
+++ b/Code Time Estimation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Steven\Target Decoy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91EA0796-5A01-4CC5-842F-632C994A5469}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BF34E90-2023-4ADD-8FFA-555B321DBEA1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2685" yWindow="1230" windowWidth="24915" windowHeight="11385" xr2:uid="{963D9261-D2CF-4690-9B13-72A79E140905}"/>
   </bookViews>
@@ -1875,7 +1875,7 @@
   <dimension ref="A1:S20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>